<commit_message>
New Writer Prototype Added
Prototype that deals with 9 out of the 10 FieldAttrTypes has been added
</commit_message>
<xml_diff>
--- a/Gannt for Field Attr Types.xlsx
+++ b/Gannt for Field Attr Types.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tasks" sheetId="1" r:id="rId1"/>
+    <sheet name="Matt Planning" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
   <si>
     <t>INTEGER</t>
   </si>
@@ -51,13 +52,136 @@
     <t>INTERVAL</t>
   </si>
   <si>
-    <t>*Red means not done, green means done</t>
-  </si>
-  <si>
     <t>Reader (Monica)</t>
   </si>
   <si>
     <t>Writer (Matthew)</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Research:</t>
+  </si>
+  <si>
+    <t>Get format string from KNIME</t>
+  </si>
+  <si>
+    <t>User must explicity define column as Unknown</t>
+  </si>
+  <si>
+    <t>User must explicity define column as Money
+(type must be double)</t>
+  </si>
+  <si>
+    <t>User must explicity define column as Timestamp
+(type must be date-time)</t>
+  </si>
+  <si>
+    <t>User must explicity define column as Real, in conjunction with nDec
+(type must be double)</t>
+  </si>
+  <si>
+    <t>User must explicity define column as FIX, in conjunction
+with nDec
+(type must be double)</t>
+  </si>
+  <si>
+    <t>Default for string type</t>
+  </si>
+  <si>
+    <t>Default for integer type</t>
+  </si>
+  <si>
+    <t>Has Format String?</t>
+  </si>
+  <si>
+    <t>Uses nDec?</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Integer, double</t>
+  </si>
+  <si>
+    <t>Integer, double, string</t>
+  </si>
+  <si>
+    <t>Local date time</t>
+  </si>
+  <si>
+    <t>Default for "local data time" type</t>
+  </si>
+  <si>
+    <t>Default for "local time" type</t>
+  </si>
+  <si>
+    <t>Local time</t>
+  </si>
+  <si>
+    <t>Allowed KNIME data types</t>
+  </si>
+  <si>
+    <t>User must explicitly define column as Interval
+Expected format: HH:MM:SS-HH:MM:SS or HH:MM-HH:MM</t>
+  </si>
+  <si>
+    <t>*Green = Done</t>
+  </si>
+  <si>
+    <t>*Yellow = Done, but unsure if implemenation is correct</t>
+  </si>
+  <si>
+    <t>*Red = Not done</t>
+  </si>
+  <si>
+    <t>Unsure of how FieldAttributes.fmt works</t>
+  </si>
+  <si>
+    <t>Unsure of what this means (what time of format string is expected here?)</t>
+  </si>
+  <si>
+    <t>Project Backlog</t>
+  </si>
+  <si>
+    <t>Deal with reloading of new csv file (specifically, FieldAttributesPanel)</t>
+  </si>
+  <si>
+    <t>User-interface clean-up</t>
+  </si>
+  <si>
+    <t>Bold column headers in UI</t>
+  </si>
+  <si>
+    <t>Hide (or disable) nDecs if its value is not relevant</t>
+  </si>
+  <si>
+    <t>Dealing with null values</t>
+  </si>
+  <si>
+    <t>Comma and thousand separator</t>
+  </si>
+  <si>
+    <t>Comments/Documentation</t>
+  </si>
+  <si>
+    <t>Integrating this code into actual KNIME code</t>
+  </si>
+  <si>
+    <t>Interval FieldAttrType</t>
+  </si>
+  <si>
+    <t>Default Table Name should be selected initially</t>
+  </si>
+  <si>
+    <t>TableHeader: Fixed Point Decimals</t>
   </si>
 </sst>
 </file>
@@ -81,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,6 +215,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -107,10 +243,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,23 +546,23 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" customWidth="1"/>
     <col min="2" max="2" width="18.21875" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+    <col min="3" max="3" width="72.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -418,23 +570,23 @@
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="C4" s="8"/>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -442,49 +594,310 @@
         <v>1</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="C5" s="8"/>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="8"/>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="C8" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="C9" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="C10" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="45.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bug fix for FieldAttrPanel
Bug fix for: FieldAttrPanel would not load the saved settings (nDec and FieldAttr) if the input Buffered Data Table was changed
</commit_message>
<xml_diff>
--- a/Gannt for Field Attr Types.xlsx
+++ b/Gannt for Field Attr Types.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t>INTEGER</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Project Backlog</t>
   </si>
   <si>
-    <t>Deal with reloading of new csv file (specifically, FieldAttributesPanel)</t>
-  </si>
-  <si>
     <t>User-interface clean-up</t>
   </si>
   <si>
@@ -178,19 +175,19 @@
     <t>Interval FieldAttrType</t>
   </si>
   <si>
-    <t>Default Table Name should be selected initially</t>
-  </si>
-  <si>
     <t>TableHeader: Fixed Point Decimals</t>
   </si>
   <si>
     <t>Add image to qvx writer node</t>
   </si>
   <si>
-    <t>To do this, store a DataTableSpec in QvxWriterNodeSettings, then when selecting nDec and FieldAttr, check if the currently loaded DataTableSpec is equal to it</t>
-  </si>
-  <si>
     <t>Did I do this correctly? Check with Monica.</t>
+  </si>
+  <si>
+    <t>Advanced Settings Panel</t>
+  </si>
+  <si>
+    <t>Image of the word "qvx"</t>
   </si>
 </sst>
 </file>
@@ -557,7 +554,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,10 +667,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -856,35 +853,31 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="E14" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="E18" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -893,12 +886,12 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="11" t="s">
         <v>48</v>
       </c>
     </row>
@@ -906,20 +899,16 @@
       <c r="A22" s="11" t="s">
         <v>49</v>
       </c>
+      <c r="E22" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>52</v>
+      <c r="E23" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added scrollbar to FieldAttrPanel
Added scrollbar to FieldAttrPanel
</commit_message>
<xml_diff>
--- a/Gannt for Field Attr Types.xlsx
+++ b/Gannt for Field Attr Types.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>INTEGER</t>
   </si>
@@ -160,9 +160,6 @@
     <t>Hide (or disable) nDecs if its value is not relevant</t>
   </si>
   <si>
-    <t>Dealing with null values</t>
-  </si>
-  <si>
     <t>Comma and thousand separator</t>
   </si>
   <si>
@@ -181,13 +178,13 @@
     <t>Add image to qvx writer node</t>
   </si>
   <si>
-    <t>Did I do this correctly? Check with Monica.</t>
-  </si>
-  <si>
     <t>Advanced Settings Panel</t>
   </si>
   <si>
     <t>Image of the word "qvx"</t>
+  </si>
+  <si>
+    <t>Add scroll bar to FieldAttrPanel</t>
   </si>
 </sst>
 </file>
@@ -270,7 +267,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -669,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,25 +865,22 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E17" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="12" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="11" t="s">
         <v>47</v>
       </c>
     </row>
@@ -894,21 +888,21 @@
       <c r="A21" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>49</v>
       </c>
       <c r="E22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Node descriptions and scrollbar added
Node descriptions for both QvxReader and QvxWriter were added. Scrollbar was added to FieldAttrPanel, so that a table with many columns does not mess up the entire UI
</commit_message>
<xml_diff>
--- a/Gannt for Field Attr Types.xlsx
+++ b/Gannt for Field Attr Types.xlsx
@@ -166,9 +166,6 @@
     <t>Comments/Documentation</t>
   </si>
   <si>
-    <t>Integrating this code into actual KNIME code</t>
-  </si>
-  <si>
     <t>Interval FieldAttrType</t>
   </si>
   <si>
@@ -184,7 +181,10 @@
     <t>Image of the word "qvx"</t>
   </si>
   <si>
-    <t>Add scroll bar to FieldAttrPanel</t>
+    <t>Write Descriptions for Advanced Panel</t>
+  </si>
+  <si>
+    <t>Reader treats different FieldAttrTypes differently</t>
   </si>
 </sst>
 </file>
@@ -246,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -268,12 +268,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9900"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -551,7 +557,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,13 +672,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="45.33203125" customWidth="1"/>
     <col min="2" max="2" width="45.44140625" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="12.109375" customWidth="1"/>
@@ -865,7 +871,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="13" t="s">
         <v>44</v>
       </c>
     </row>
@@ -875,17 +881,20 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="11" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="13" t="s">
         <v>47</v>
       </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E21" t="s">
@@ -893,10 +902,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="A22" s="12" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Handling of additional FieldAttrTypes
Qvx Reader handles more FieldAttrTypes, FixPointDecimals.  Rewriting of Reader documentation.
</commit_message>
<xml_diff>
--- a/Gannt for Field Attr Types.xlsx
+++ b/Gannt for Field Attr Types.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>INTEGER</t>
   </si>
@@ -50,12 +50,6 @@
   </si>
   <si>
     <t>INTERVAL</t>
-  </si>
-  <si>
-    <t>Reader (Monica)</t>
-  </si>
-  <si>
-    <t>Writer (Matthew)</t>
   </si>
   <si>
     <t>Integer</t>
@@ -176,6 +170,15 @@
   </si>
   <si>
     <t>Reader treats different FieldAttrTypes differently</t>
+  </si>
+  <si>
+    <t>Reader</t>
+  </si>
+  <si>
+    <t>Writer</t>
+  </si>
+  <si>
+    <t>Reg-exp function</t>
   </si>
 </sst>
 </file>
@@ -547,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,97 +564,105 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="C8" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="C9" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="C10" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="C11" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -663,7 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -679,16 +690,16 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -696,12 +707,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -709,12 +720,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -722,12 +733,12 @@
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -735,14 +746,14 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -750,17 +761,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -768,17 +779,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -786,14 +797,14 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -801,14 +812,14 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -816,14 +827,14 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -831,62 +842,62 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Qvx Reader update in progress
In the process of reading Date/Time/Timestamp/Interval values
</commit_message>
<xml_diff>
--- a/Gannt for Field Attr Types.xlsx
+++ b/Gannt for Field Attr Types.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>INTEGER</t>
   </si>
@@ -136,12 +136,6 @@
     <t>*Red = Not done</t>
   </si>
   <si>
-    <t>Unsure of how FieldAttributes.fmt works</t>
-  </si>
-  <si>
-    <t>Unsure of what this means (what time of format string is expected here?)</t>
-  </si>
-  <si>
     <t>Project Backlog</t>
   </si>
   <si>
@@ -179,6 +173,18 @@
   </si>
   <si>
     <t>Reg-exp function</t>
+  </si>
+  <si>
+    <t>M/D/YYYY</t>
+  </si>
+  <si>
+    <t>h:mm:ss TT</t>
+  </si>
+  <si>
+    <t>M/D/YYYY h:mm:ss[.fff] TT</t>
+  </si>
+  <si>
+    <t>Unsure of how to use Excel to generate this data type</t>
   </si>
 </sst>
 </file>
@@ -240,9 +246,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -257,12 +262,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,7 +556,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,107 +567,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>49</v>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
       <c r="E4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
       <c r="E5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
       <c r="E6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -688,68 +693,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
       <c r="E2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
       <c r="E3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
       <c r="E4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
@@ -757,14 +762,14 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="s">
@@ -775,16 +780,16 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="4"/>
       <c r="E7" t="s">
         <v>25</v>
       </c>
@@ -793,111 +798,111 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="4"/>
       <c r="E8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="4"/>
       <c r="E9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="4"/>
       <c r="E10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="4"/>
       <c r="E11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+      <c r="E19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E19" t="s">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reader now reads dates
Reader now reads dates
</commit_message>
<xml_diff>
--- a/Gannt for Field Attr Types.xlsx
+++ b/Gannt for Field Attr Types.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t>INTEGER</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Unsure of how to use Excel to generate this data type</t>
+  </si>
+  <si>
+    <t>Deprecated version of DateAndTimeCell</t>
   </si>
 </sst>
 </file>
@@ -223,13 +226,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -261,13 +264,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,13 +559,13 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" customWidth="1"/>
     <col min="3" max="3" width="72.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -579,22 +582,22 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
       <c r="E4" t="s">
         <v>33</v>
       </c>
@@ -603,8 +606,8 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
       <c r="E5" t="s">
         <v>34</v>
       </c>
@@ -613,8 +616,8 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
       <c r="E6" t="s">
         <v>35</v>
       </c>
@@ -623,17 +626,17 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>49</v>
       </c>
     </row>
@@ -641,10 +644,10 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -652,10 +655,10 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -663,10 +666,10 @@
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>50</v>
       </c>
     </row>
@@ -868,27 +871,27 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>42</v>
       </c>
       <c r="E19" t="s">
@@ -896,12 +899,12 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Writer works for 9 out of 10 types
Writer works for every type except Time
</commit_message>
<xml_diff>
--- a/Gannt for Field Attr Types.xlsx
+++ b/Gannt for Field Attr Types.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>INTEGER</t>
   </si>
@@ -172,25 +172,25 @@
     <t>Writer</t>
   </si>
   <si>
-    <t>Reg-exp function</t>
-  </si>
-  <si>
-    <t>M/D/YYYY</t>
-  </si>
-  <si>
-    <t>h:mm:ss TT</t>
-  </si>
-  <si>
-    <t>M/D/YYYY h:mm:ss[.fff] TT</t>
-  </si>
-  <si>
-    <t>Unsure of how to use Excel to generate this data type</t>
-  </si>
-  <si>
-    <t>Deprecated version of DateAndTimeCell</t>
-  </si>
-  <si>
     <t>Any dates before Feb 28, 1900 are one day off</t>
+  </si>
+  <si>
+    <t>Timestamp format (figure out how to generate in QlikView)</t>
+  </si>
+  <si>
+    <t>Reader + Writer: Null values should be allowed for QvxSpecialExtent, LocalDateTime, LocalDate, etc.</t>
+  </si>
+  <si>
+    <t>Deprecated verison of DateAndTimeCell</t>
+  </si>
+  <si>
+    <t>Writer: Support for LocalDateTime, LocalDate, etc cell types</t>
+  </si>
+  <si>
+    <t>Unsure of how to use Excel + QlikView to generate this data type</t>
+  </si>
+  <si>
+    <t>Things to Do</t>
   </si>
 </sst>
 </file>
@@ -270,10 +270,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,22 +585,22 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
       <c r="E4" t="s">
         <v>33</v>
       </c>
@@ -609,8 +609,8 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
       <c r="E5" t="s">
         <v>34</v>
       </c>
@@ -619,8 +619,8 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
       <c r="E6" t="s">
         <v>35</v>
       </c>
@@ -629,56 +629,67 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>51</v>
-      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
-        <v>54</v>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -691,7 +702,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
JAXB Generation Project added
This project demonstrates how we generated the JAXB classes that we used in our QvxReader and QvxWriter projects.
</commit_message>
<xml_diff>
--- a/Gannt for Field Attr Types.xlsx
+++ b/Gannt for Field Attr Types.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Any dates before Feb 28, 1900 are one day off</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Monica</t>
-  </si>
-  <si>
-    <t>Testing process</t>
   </si>
   <si>
     <t>Function we talked about</t>
@@ -470,7 +467,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,13 +489,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -521,31 +518,23 @@
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -553,100 +542,102 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
         <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
         <v>25</v>
-      </c>
-      <c r="H13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>